<commit_message>
Adding cover data for RainShelter trial
</commit_message>
<xml_diff>
--- a/Prototypes/Oats/Observed.xlsx
+++ b/Prototypes/Oats/Observed.xlsx
@@ -1205,6 +1205,9 @@
       <c r="AM2">
         <v>0</v>
       </c>
+      <c r="AO2">
+        <v>0.408330493856865</v>
+      </c>
       <c r="AP2">
         <v>0</v>
       </c>
@@ -1333,6 +1336,9 @@
       <c r="AM3">
         <v>0</v>
       </c>
+      <c r="AO3">
+        <v>0.700852190433432</v>
+      </c>
       <c r="AP3">
         <v>0.15</v>
       </c>
@@ -1461,6 +1467,9 @@
       <c r="AM4">
         <v>0</v>
       </c>
+      <c r="AO4">
+        <v>0.820426025367115</v>
+      </c>
       <c r="AP4">
         <v>0.08</v>
       </c>
@@ -1589,6 +1598,9 @@
       <c r="AM5">
         <v>0</v>
       </c>
+      <c r="AO5">
+        <v>0.916509206348116</v>
+      </c>
       <c r="AP5">
         <v>0.52</v>
       </c>
@@ -1678,6 +1690,9 @@
       <c r="AM6">
         <v>0</v>
       </c>
+      <c r="AO6">
+        <v>0.980468082947382</v>
+      </c>
       <c r="AP6">
         <v>1.36</v>
       </c>
@@ -1722,6 +1737,9 @@
       <c r="AM7">
         <v>0</v>
       </c>
+      <c r="AO7">
+        <v>0.971369199682235</v>
+      </c>
       <c r="AP7">
         <v>1.88</v>
       </c>
@@ -1850,6 +1868,9 @@
       <c r="AN8">
         <v>64.94</v>
       </c>
+      <c r="AO8">
+        <v>0.976636310477213</v>
+      </c>
       <c r="AP8">
         <v>3.17</v>
       </c>
@@ -1975,6 +1996,9 @@
       <c r="AN9">
         <v>162.42</v>
       </c>
+      <c r="AO9">
+        <v>0.972035304022243</v>
+      </c>
       <c r="AP9">
         <v>4.62</v>
       </c>
@@ -2097,6 +2121,9 @@
       <c r="AN10">
         <v>238.62</v>
       </c>
+      <c r="AO10">
+        <v>0.855097674900448</v>
+      </c>
       <c r="AP10">
         <v>6.37</v>
       </c>
@@ -2150,6 +2177,9 @@
       <c r="AN11">
         <v>470.95</v>
       </c>
+      <c r="AO11">
+        <v>0.778953634254409</v>
+      </c>
       <c r="AP11">
         <v>6.09</v>
       </c>
@@ -2203,6 +2233,9 @@
       <c r="AN12">
         <v>559.24</v>
       </c>
+      <c r="AO12">
+        <v>0.876380533909057</v>
+      </c>
       <c r="AP12">
         <v>9.4</v>
       </c>
@@ -2322,6 +2355,9 @@
       <c r="AN13">
         <v>753.01</v>
       </c>
+      <c r="AO13">
+        <v>0.813356867580697</v>
+      </c>
       <c r="AP13">
         <v>9.48</v>
       </c>
@@ -2441,6 +2477,9 @@
       <c r="AN14">
         <v>988.88</v>
       </c>
+      <c r="AO14">
+        <v>0.759981414131874</v>
+      </c>
       <c r="AP14">
         <v>9.01</v>
       </c>
@@ -2491,6 +2530,9 @@
       <c r="AN15">
         <v>923.26</v>
       </c>
+      <c r="AO15">
+        <v>0.711190656386232</v>
+      </c>
       <c r="AP15">
         <v>14.77</v>
       </c>
@@ -2541,6 +2583,9 @@
       <c r="AN16">
         <v>818.78</v>
       </c>
+      <c r="AO16">
+        <v>0.68867338509175</v>
+      </c>
       <c r="AP16">
         <v>12.99</v>
       </c>
@@ -2657,6 +2702,9 @@
       <c r="AN17">
         <v>907.11</v>
       </c>
+      <c r="AO17">
+        <v>0.713234713664203</v>
+      </c>
       <c r="AP17">
         <v>13.26</v>
       </c>
@@ -2773,6 +2821,9 @@
       <c r="AN18">
         <v>852.73</v>
       </c>
+      <c r="AO18">
+        <v>0.410751134646202</v>
+      </c>
       <c r="AP18">
         <v>18.9</v>
       </c>
@@ -2886,6 +2937,9 @@
       <c r="AN19">
         <v>902.33</v>
       </c>
+      <c r="AO19">
+        <v>0.580553465079451</v>
+      </c>
       <c r="AP19">
         <v>21.71</v>
       </c>
@@ -2936,6 +2990,9 @@
       <c r="AM20">
         <v>0</v>
       </c>
+      <c r="AO20">
+        <v>0.428715369585067</v>
+      </c>
       <c r="AP20">
         <v>0</v>
       </c>
@@ -3064,6 +3121,9 @@
       <c r="AM21">
         <v>0</v>
       </c>
+      <c r="AO21">
+        <v>0.749813786257267</v>
+      </c>
       <c r="AP21">
         <v>0.09</v>
       </c>
@@ -3192,6 +3252,9 @@
       <c r="AM22">
         <v>0</v>
       </c>
+      <c r="AO22">
+        <v>0.864403074192053</v>
+      </c>
       <c r="AP22">
         <v>0.27</v>
       </c>
@@ -3320,6 +3383,9 @@
       <c r="AM23">
         <v>0</v>
       </c>
+      <c r="AO23">
+        <v>0.913781052696267</v>
+      </c>
       <c r="AP23">
         <v>0.98</v>
       </c>
@@ -3409,6 +3475,9 @@
       <c r="AM24">
         <v>0</v>
       </c>
+      <c r="AO24">
+        <v>0.934558960630851</v>
+      </c>
       <c r="AP24">
         <v>1.54</v>
       </c>
@@ -3456,6 +3525,9 @@
       <c r="AM25">
         <v>0</v>
       </c>
+      <c r="AO25">
+        <v>0.899523431795675</v>
+      </c>
       <c r="AP25">
         <v>1.35</v>
       </c>
@@ -3590,6 +3662,9 @@
       <c r="AN26">
         <v>112.69</v>
       </c>
+      <c r="AO26">
+        <v>0.9482050667135</v>
+      </c>
       <c r="AP26">
         <v>1.35</v>
       </c>
@@ -3718,6 +3793,9 @@
       <c r="AN27">
         <v>186.41</v>
       </c>
+      <c r="AO27">
+        <v>0.970619080764376</v>
+      </c>
       <c r="AP27">
         <v>4.24</v>
       </c>
@@ -3843,6 +3921,9 @@
       <c r="AN28">
         <v>270.6</v>
       </c>
+      <c r="AO28">
+        <v>0.812986008027909</v>
+      </c>
       <c r="AP28">
         <v>3.77</v>
       </c>
@@ -3896,6 +3977,9 @@
       <c r="AN29">
         <v>496.58</v>
       </c>
+      <c r="AO29">
+        <v>0.84720824024332</v>
+      </c>
       <c r="AP29">
         <v>6.42</v>
       </c>
@@ -3949,6 +4033,9 @@
       <c r="AN30">
         <v>637.15</v>
       </c>
+      <c r="AO30">
+        <v>0.848576537848046</v>
+      </c>
       <c r="AP30">
         <v>9.83</v>
       </c>
@@ -4071,6 +4158,9 @@
       <c r="AN31">
         <v>805.88</v>
       </c>
+      <c r="AO31">
+        <v>0.766101956645606</v>
+      </c>
       <c r="AP31">
         <v>9.96</v>
       </c>
@@ -4190,6 +4280,9 @@
       <c r="AN32">
         <v>759.51</v>
       </c>
+      <c r="AO32">
+        <v>0.811060324887604</v>
+      </c>
       <c r="AP32">
         <v>5.91</v>
       </c>
@@ -4240,6 +4333,9 @@
       <c r="AN33">
         <v>970.12</v>
       </c>
+      <c r="AO33">
+        <v>0.701700529771294</v>
+      </c>
       <c r="AP33">
         <v>6.25</v>
       </c>
@@ -4290,6 +4386,9 @@
       <c r="AN34">
         <v>941.94</v>
       </c>
+      <c r="AO34">
+        <v>0.730081991445581</v>
+      </c>
       <c r="AP34">
         <v>8.74</v>
       </c>
@@ -4409,6 +4508,9 @@
       <c r="AN35">
         <v>788.93</v>
       </c>
+      <c r="AO35">
+        <v>0.700673229808187</v>
+      </c>
       <c r="AP35">
         <v>5.68</v>
       </c>
@@ -4525,6 +4627,9 @@
       <c r="AN36">
         <v>992.4</v>
       </c>
+      <c r="AO36">
+        <v>0.606587409625806</v>
+      </c>
       <c r="AP36">
         <v>16.84</v>
       </c>
@@ -4644,6 +4749,9 @@
       <c r="AN37">
         <v>721.89</v>
       </c>
+      <c r="AO37">
+        <v>0.588968794338931</v>
+      </c>
       <c r="AP37">
         <v>16.8</v>
       </c>
@@ -4694,6 +4802,9 @@
       <c r="AM38">
         <v>0</v>
       </c>
+      <c r="AO38">
+        <v>0.334966697681939</v>
+      </c>
       <c r="AP38">
         <v>0</v>
       </c>
@@ -4822,6 +4933,9 @@
       <c r="AM39">
         <v>0</v>
       </c>
+      <c r="AO39">
+        <v>0.608497021183093</v>
+      </c>
       <c r="AP39">
         <v>0.05</v>
       </c>
@@ -4950,6 +5064,9 @@
       <c r="AM40">
         <v>0</v>
       </c>
+      <c r="AO40">
+        <v>0.768243246294892</v>
+      </c>
       <c r="AP40">
         <v>0.37</v>
       </c>
@@ -5078,6 +5195,9 @@
       <c r="AM41">
         <v>0</v>
       </c>
+      <c r="AO41">
+        <v>0.873244980487694</v>
+      </c>
       <c r="AP41">
         <v>0.68</v>
       </c>
@@ -5167,6 +5287,9 @@
       <c r="AM42">
         <v>0</v>
       </c>
+      <c r="AO42">
+        <v>0.89243045148372</v>
+      </c>
       <c r="AP42">
         <v>1.86</v>
       </c>
@@ -5214,6 +5337,9 @@
       <c r="AM43">
         <v>0</v>
       </c>
+      <c r="AO43">
+        <v>0.885470989351718</v>
+      </c>
       <c r="AP43">
         <v>3.28</v>
       </c>
@@ -5342,6 +5468,9 @@
       <c r="AN44">
         <v>106.81</v>
       </c>
+      <c r="AO44">
+        <v>0.838404567603578</v>
+      </c>
       <c r="AP44">
         <v>5.82</v>
       </c>
@@ -5467,6 +5596,9 @@
       <c r="AN45">
         <v>168.31</v>
       </c>
+      <c r="AO45">
+        <v>0.879791777374539</v>
+      </c>
       <c r="AP45">
         <v>6.09</v>
       </c>
@@ -5592,6 +5724,9 @@
       <c r="AN46">
         <v>275.59</v>
       </c>
+      <c r="AO46">
+        <v>0.832427789482671</v>
+      </c>
       <c r="AP46">
         <v>8.19</v>
       </c>
@@ -5645,6 +5780,9 @@
       <c r="AN47">
         <v>428.14</v>
       </c>
+      <c r="AO47">
+        <v>0.781910641116675</v>
+      </c>
       <c r="AP47">
         <v>9.48</v>
       </c>
@@ -5698,6 +5836,9 @@
       <c r="AN48">
         <v>566.27</v>
       </c>
+      <c r="AO48">
+        <v>0.873122673453369</v>
+      </c>
       <c r="AP48">
         <v>10</v>
       </c>
@@ -5823,6 +5964,9 @@
       <c r="AN49">
         <v>856.73</v>
       </c>
+      <c r="AO49">
+        <v>0.840756234555947</v>
+      </c>
       <c r="AP49">
         <v>5.32</v>
       </c>
@@ -5942,6 +6086,9 @@
       <c r="AN50">
         <v>674.21</v>
       </c>
+      <c r="AO50">
+        <v>0.728436456553553</v>
+      </c>
       <c r="AP50">
         <v>4.53</v>
       </c>
@@ -5992,6 +6139,9 @@
       <c r="AN51">
         <v>696.73</v>
       </c>
+      <c r="AO51">
+        <v>0.776884949900945</v>
+      </c>
       <c r="AP51">
         <v>6.45</v>
       </c>
@@ -6042,6 +6192,9 @@
       <c r="AN52">
         <v>1046.99</v>
       </c>
+      <c r="AO52">
+        <v>0.855604012865153</v>
+      </c>
       <c r="AP52">
         <v>4.8</v>
       </c>
@@ -6161,6 +6314,9 @@
       <c r="AN53">
         <v>784.37</v>
       </c>
+      <c r="AO53">
+        <v>0.696523835478193</v>
+      </c>
       <c r="AP53">
         <v>3.02</v>
       </c>
@@ -6277,6 +6433,9 @@
       <c r="AN54">
         <v>1147.39</v>
       </c>
+      <c r="AO54">
+        <v>0.694508723279635</v>
+      </c>
       <c r="AP54">
         <v>8.95</v>
       </c>
@@ -6393,6 +6552,9 @@
       <c r="AN55">
         <v>694.53</v>
       </c>
+      <c r="AO55">
+        <v>0.80308059736441</v>
+      </c>
       <c r="AP55">
         <v>7.11</v>
       </c>
@@ -6443,6 +6605,9 @@
       <c r="AM56">
         <v>0</v>
       </c>
+      <c r="AO56">
+        <v>0.2953330976898</v>
+      </c>
       <c r="AP56">
         <v>0</v>
       </c>
@@ -6571,6 +6736,9 @@
       <c r="AM57">
         <v>0</v>
       </c>
+      <c r="AO57">
+        <v>0.532604938449706</v>
+      </c>
       <c r="AP57">
         <v>0.08</v>
       </c>
@@ -6699,6 +6867,9 @@
       <c r="AM58">
         <v>0</v>
       </c>
+      <c r="AO58">
+        <v>0.83185756165124</v>
+      </c>
       <c r="AP58">
         <v>0.03</v>
       </c>
@@ -6827,6 +6998,9 @@
       <c r="AM59">
         <v>0</v>
       </c>
+      <c r="AO59">
+        <v>0.872732650863372</v>
+      </c>
       <c r="AP59">
         <v>0.44</v>
       </c>
@@ -6916,6 +7090,9 @@
       <c r="AM60">
         <v>0</v>
       </c>
+      <c r="AO60">
+        <v>0.905289955333571</v>
+      </c>
       <c r="AP60">
         <v>0.77</v>
       </c>
@@ -6963,6 +7140,9 @@
       <c r="AM61">
         <v>0</v>
       </c>
+      <c r="AO61">
+        <v>0.859912000006647</v>
+      </c>
       <c r="AP61">
         <v>3.44</v>
       </c>
@@ -7094,6 +7274,9 @@
       <c r="AN62">
         <v>103.72</v>
       </c>
+      <c r="AO62">
+        <v>0.864746098287556</v>
+      </c>
       <c r="AP62">
         <v>3.64</v>
       </c>
@@ -7216,6 +7399,9 @@
       <c r="AN63">
         <v>164.36</v>
       </c>
+      <c r="AO63">
+        <v>0.800639615690768</v>
+      </c>
       <c r="AP63">
         <v>8.84</v>
       </c>
@@ -7338,6 +7524,9 @@
       <c r="AN64">
         <v>214.87</v>
       </c>
+      <c r="AO64">
+        <v>0.643177456618168</v>
+      </c>
       <c r="AP64">
         <v>8.87</v>
       </c>
@@ -7391,6 +7580,9 @@
       <c r="AN65">
         <v>473.38</v>
       </c>
+      <c r="AO65">
+        <v>0.630181591171395</v>
+      </c>
       <c r="AP65">
         <v>13.51</v>
       </c>
@@ -7444,6 +7636,9 @@
       <c r="AN66">
         <v>612.55</v>
       </c>
+      <c r="AO66">
+        <v>0.773558892454322</v>
+      </c>
       <c r="AP66">
         <v>11.95</v>
       </c>
@@ -7563,6 +7758,9 @@
       <c r="AN67">
         <v>628.65</v>
       </c>
+      <c r="AO67">
+        <v>0.653504319366203</v>
+      </c>
       <c r="AP67">
         <v>6.86</v>
       </c>
@@ -7679,6 +7877,9 @@
       <c r="AN68">
         <v>738.72</v>
       </c>
+      <c r="AO68">
+        <v>0.749200108934315</v>
+      </c>
       <c r="AP68">
         <v>6.52</v>
       </c>
@@ -7729,6 +7930,9 @@
       <c r="AN69">
         <v>779.52</v>
       </c>
+      <c r="AO69">
+        <v>0.710581685545635</v>
+      </c>
       <c r="AP69">
         <v>6.56</v>
       </c>
@@ -7779,6 +7983,9 @@
       <c r="AN70">
         <v>808.96</v>
       </c>
+      <c r="AO70">
+        <v>0.703040644936197</v>
+      </c>
       <c r="AP70">
         <v>3.67</v>
       </c>
@@ -7898,6 +8105,9 @@
       <c r="AN71">
         <v>809.34</v>
       </c>
+      <c r="AO71">
+        <v>0.665789621203423</v>
+      </c>
       <c r="AP71">
         <v>4.65</v>
       </c>
@@ -8014,6 +8224,9 @@
       <c r="AN72">
         <v>923.51</v>
       </c>
+      <c r="AO72">
+        <v>0.725775743157166</v>
+      </c>
       <c r="AP72">
         <v>4.6</v>
       </c>
@@ -8130,6 +8343,9 @@
       <c r="AN73">
         <v>573.59</v>
       </c>
+      <c r="AO73">
+        <v>0.588297410754662</v>
+      </c>
       <c r="AP73">
         <v>7.02</v>
       </c>
@@ -8180,6 +8396,9 @@
       <c r="AM74">
         <v>0</v>
       </c>
+      <c r="AO74">
+        <v>0.328854006346898</v>
+      </c>
       <c r="AP74">
         <v>0</v>
       </c>
@@ -8308,6 +8527,9 @@
       <c r="AM75">
         <v>0</v>
       </c>
+      <c r="AO75">
+        <v>0.713741828013774</v>
+      </c>
       <c r="AP75">
         <v>0.12</v>
       </c>
@@ -8436,6 +8658,9 @@
       <c r="AM76">
         <v>0</v>
       </c>
+      <c r="AO76">
+        <v>0.889493288838129</v>
+      </c>
       <c r="AP76">
         <v>0.18</v>
       </c>
@@ -8564,6 +8789,9 @@
       <c r="AM77">
         <v>0</v>
       </c>
+      <c r="AO77">
+        <v>0.978887852751892</v>
+      </c>
       <c r="AP77">
         <v>0.73</v>
       </c>
@@ -8653,6 +8881,9 @@
       <c r="AM78">
         <v>0</v>
       </c>
+      <c r="AO78">
+        <v>0.988900223006712</v>
+      </c>
       <c r="AP78">
         <v>3.28</v>
       </c>
@@ -8694,6 +8925,9 @@
       <c r="AM79">
         <v>0</v>
       </c>
+      <c r="AO79">
+        <v>0.985861645750459</v>
+      </c>
       <c r="AP79">
         <v>3.84</v>
       </c>
@@ -8819,6 +9053,9 @@
       <c r="AN80">
         <v>7.46</v>
       </c>
+      <c r="AO80">
+        <v>0.964096370170566</v>
+      </c>
       <c r="AP80">
         <v>6.09</v>
       </c>
@@ -8941,6 +9178,9 @@
       <c r="AN81">
         <v>87.3</v>
       </c>
+      <c r="AO81">
+        <v>0.971155667033882</v>
+      </c>
       <c r="AP81">
         <v>9.8</v>
       </c>
@@ -9063,6 +9303,9 @@
       <c r="AN82">
         <v>165.85</v>
       </c>
+      <c r="AO82">
+        <v>0.919987316752223</v>
+      </c>
       <c r="AP82">
         <v>7.26</v>
       </c>
@@ -9110,6 +9353,9 @@
       <c r="AN83">
         <v>337.81</v>
       </c>
+      <c r="AO83">
+        <v>0.915965261339335</v>
+      </c>
       <c r="AP83">
         <v>10.46</v>
       </c>
@@ -9163,6 +9409,9 @@
       <c r="AN84">
         <v>533.62</v>
       </c>
+      <c r="AO84">
+        <v>0.887026437614795</v>
+      </c>
       <c r="AP84">
         <v>11.56</v>
       </c>
@@ -9282,6 +9531,9 @@
       <c r="AN85">
         <v>841.49</v>
       </c>
+      <c r="AO85">
+        <v>0.889279501763975</v>
+      </c>
       <c r="AP85">
         <v>13.12</v>
       </c>
@@ -9401,6 +9653,9 @@
       <c r="AN86">
         <v>701.97</v>
       </c>
+      <c r="AO86">
+        <v>0.853691529766432</v>
+      </c>
       <c r="AP86">
         <v>7.82</v>
       </c>
@@ -9451,6 +9706,9 @@
       <c r="AN87">
         <v>804.79</v>
       </c>
+      <c r="AO87">
+        <v>0.853240290579619</v>
+      </c>
       <c r="AP87">
         <v>16.25</v>
       </c>
@@ -9501,6 +9759,9 @@
       <c r="AN88">
         <v>807.37</v>
       </c>
+      <c r="AO88">
+        <v>0.734875299460241</v>
+      </c>
       <c r="AP88">
         <v>21.95</v>
       </c>
@@ -9614,6 +9875,9 @@
       <c r="AN89">
         <v>912.98</v>
       </c>
+      <c r="AO89">
+        <v>0.727967176800942</v>
+      </c>
       <c r="AP89">
         <v>25.57</v>
       </c>
@@ -9724,6 +9988,9 @@
       <c r="AN90">
         <v>648.3</v>
       </c>
+      <c r="AO90">
+        <v>0.338387094939096</v>
+      </c>
       <c r="AP90">
         <v>31.16</v>
       </c>
@@ -9837,6 +10104,9 @@
       <c r="AN91">
         <v>679.55</v>
       </c>
+      <c r="AO91">
+        <v>0.420739111333983</v>
+      </c>
       <c r="AP91">
         <v>29.56</v>
       </c>
@@ -9884,6 +10154,9 @@
       <c r="AM92">
         <v>0</v>
       </c>
+      <c r="AO92">
+        <v>0.334247571375451</v>
+      </c>
       <c r="AP92">
         <v>0</v>
       </c>
@@ -10012,6 +10285,9 @@
       <c r="AM93">
         <v>0</v>
       </c>
+      <c r="AO93">
+        <v>0.693074351802596</v>
+      </c>
       <c r="AP93">
         <v>0.1</v>
       </c>
@@ -10140,6 +10416,9 @@
       <c r="AM94">
         <v>0</v>
       </c>
+      <c r="AO94">
+        <v>0.830532601934153</v>
+      </c>
       <c r="AP94">
         <v>0.09</v>
       </c>
@@ -10268,6 +10547,9 @@
       <c r="AM95">
         <v>0</v>
       </c>
+      <c r="AO95">
+        <v>0.931045952955024</v>
+      </c>
       <c r="AP95">
         <v>0.69</v>
       </c>
@@ -10357,6 +10639,9 @@
       <c r="AM96">
         <v>0</v>
       </c>
+      <c r="AO96">
+        <v>0.950630013412726</v>
+      </c>
       <c r="AP96">
         <v>1.2</v>
       </c>
@@ -10404,6 +10689,9 @@
       <c r="AM97">
         <v>0</v>
       </c>
+      <c r="AO97">
+        <v>0.922479093547034</v>
+      </c>
       <c r="AP97">
         <v>3.94</v>
       </c>
@@ -10532,6 +10820,9 @@
       <c r="AN98">
         <v>90.82</v>
       </c>
+      <c r="AO98">
+        <v>0.875465359580516</v>
+      </c>
       <c r="AP98">
         <v>6.08</v>
       </c>
@@ -10654,6 +10945,9 @@
       <c r="AN99">
         <v>165.33</v>
       </c>
+      <c r="AO99">
+        <v>0.860406762775734</v>
+      </c>
       <c r="AP99">
         <v>10.73</v>
       </c>
@@ -10773,6 +11067,9 @@
       <c r="AN100">
         <v>314.81</v>
       </c>
+      <c r="AO100">
+        <v>0.793488471175513</v>
+      </c>
       <c r="AP100">
         <v>17.87</v>
       </c>
@@ -10826,6 +11123,9 @@
       <c r="AN101">
         <v>424.57</v>
       </c>
+      <c r="AO101">
+        <v>0.657949223076854</v>
+      </c>
       <c r="AP101">
         <v>23.66</v>
       </c>
@@ -10879,6 +11179,9 @@
       <c r="AN102">
         <v>476.6</v>
       </c>
+      <c r="AO102">
+        <v>0</v>
+      </c>
       <c r="AP102">
         <v>31.32</v>
       </c>
@@ -10983,6 +11286,9 @@
       <c r="AN103">
         <v>634.51</v>
       </c>
+      <c r="AO103">
+        <v>0</v>
+      </c>
       <c r="AP103">
         <v>117.62</v>
       </c>
@@ -11084,6 +11390,9 @@
       <c r="AN104">
         <v>577.24</v>
       </c>
+      <c r="AO104">
+        <v>0</v>
+      </c>
       <c r="AP104">
         <v>94.95</v>
       </c>
@@ -11131,6 +11440,9 @@
       <c r="AN105">
         <v>574.52</v>
       </c>
+      <c r="AO105">
+        <v>0</v>
+      </c>
       <c r="AP105">
         <v>92.45</v>
       </c>
@@ -11175,6 +11487,9 @@
       <c r="AN106">
         <v>507.33</v>
       </c>
+      <c r="AO106">
+        <v>0</v>
+      </c>
       <c r="AQ106">
         <v>9</v>
       </c>
@@ -11258,6 +11573,9 @@
       <c r="AM107">
         <v>0</v>
       </c>
+      <c r="AO107">
+        <v>0</v>
+      </c>
       <c r="AQ107">
         <v>9</v>
       </c>
@@ -11338,6 +11656,9 @@
       <c r="AM108">
         <v>0</v>
       </c>
+      <c r="AO108">
+        <v>0</v>
+      </c>
       <c r="AQ108">
         <v>9</v>
       </c>
@@ -11418,6 +11739,9 @@
       <c r="AM109">
         <v>0</v>
       </c>
+      <c r="AO109">
+        <v>0</v>
+      </c>
       <c r="AQ109">
         <v>9</v>
       </c>
@@ -11447,6 +11771,9 @@
       <c r="AM110">
         <v>0</v>
       </c>
+      <c r="AO110">
+        <v>0.429482812639979</v>
+      </c>
       <c r="AP110">
         <v>0</v>
       </c>
@@ -11575,6 +11902,9 @@
       <c r="AM111">
         <v>0</v>
       </c>
+      <c r="AO111">
+        <v>0.746765700599588</v>
+      </c>
       <c r="AP111">
         <v>0.17</v>
       </c>
@@ -11703,6 +12033,9 @@
       <c r="AM112">
         <v>0</v>
       </c>
+      <c r="AO112">
+        <v>0.949860158164024</v>
+      </c>
       <c r="AP112">
         <v>0.49</v>
       </c>
@@ -11831,6 +12164,9 @@
       <c r="AM113">
         <v>0</v>
       </c>
+      <c r="AO113">
+        <v>0.979690599829515</v>
+      </c>
       <c r="AP113">
         <v>1.2</v>
       </c>
@@ -11920,6 +12256,9 @@
       <c r="AM114">
         <v>0</v>
       </c>
+      <c r="AO114">
+        <v>0.986360615901761</v>
+      </c>
       <c r="AP114">
         <v>2.63</v>
       </c>
@@ -11964,6 +12303,9 @@
       <c r="AM115">
         <v>0</v>
       </c>
+      <c r="AO115">
+        <v>0.942447253670511</v>
+      </c>
       <c r="AP115">
         <v>8.4</v>
       </c>
@@ -12089,6 +12431,9 @@
       <c r="AN116">
         <v>76.58</v>
       </c>
+      <c r="AO116">
+        <v>0.94849312628949</v>
+      </c>
       <c r="AP116">
         <v>13.21</v>
       </c>
@@ -12208,6 +12553,9 @@
       <c r="AN117">
         <v>138.52</v>
       </c>
+      <c r="AO117">
+        <v>0.913674740276466</v>
+      </c>
       <c r="AP117">
         <v>17.95</v>
       </c>
@@ -12327,6 +12675,9 @@
       <c r="AN118">
         <v>258.15</v>
       </c>
+      <c r="AO118">
+        <v>0.833704002239914</v>
+      </c>
       <c r="AP118">
         <v>28.17</v>
       </c>
@@ -12380,6 +12731,9 @@
       <c r="AN119">
         <v>404.98</v>
       </c>
+      <c r="AO119">
+        <v>0.767662014893696</v>
+      </c>
       <c r="AP119">
         <v>37.89</v>
       </c>
@@ -12433,6 +12787,9 @@
       <c r="AN120">
         <v>597.15</v>
       </c>
+      <c r="AO120">
+        <v>0.315741562369824</v>
+      </c>
       <c r="AP120">
         <v>41.46</v>
       </c>
@@ -12540,6 +12897,9 @@
       <c r="AN121">
         <v>686.02</v>
       </c>
+      <c r="AO121">
+        <v>0</v>
+      </c>
       <c r="AP121">
         <v>125.63</v>
       </c>
@@ -12641,6 +13001,9 @@
       <c r="AN122">
         <v>661.07</v>
       </c>
+      <c r="AO122">
+        <v>0</v>
+      </c>
       <c r="AP122">
         <v>123.88</v>
       </c>
@@ -12688,6 +13051,9 @@
       <c r="AN123">
         <v>654.45</v>
       </c>
+      <c r="AO123">
+        <v>0</v>
+      </c>
       <c r="AP123">
         <v>115.2</v>
       </c>
@@ -12732,6 +13098,9 @@
       <c r="AN124">
         <v>543.06</v>
       </c>
+      <c r="AO124">
+        <v>0</v>
+      </c>
       <c r="AQ124">
         <v>9</v>
       </c>
@@ -12815,6 +13184,9 @@
       <c r="AM125">
         <v>0</v>
       </c>
+      <c r="AO125">
+        <v>0</v>
+      </c>
       <c r="AQ125">
         <v>9</v>
       </c>
@@ -12895,6 +13267,9 @@
       <c r="AM126">
         <v>0</v>
       </c>
+      <c r="AO126">
+        <v>0</v>
+      </c>
       <c r="AQ126">
         <v>9</v>
       </c>
@@ -12975,6 +13350,9 @@
       <c r="AM127">
         <v>0</v>
       </c>
+      <c r="AO127">
+        <v>0</v>
+      </c>
       <c r="AQ127">
         <v>9</v>
       </c>
@@ -13004,6 +13382,9 @@
       <c r="AM128">
         <v>0</v>
       </c>
+      <c r="AO128">
+        <v>0.393621744645719</v>
+      </c>
       <c r="AP128">
         <v>0</v>
       </c>
@@ -13132,6 +13513,9 @@
       <c r="AM129">
         <v>0</v>
       </c>
+      <c r="AO129">
+        <v>0.715491677552311</v>
+      </c>
       <c r="AP129">
         <v>0.12</v>
       </c>
@@ -13260,6 +13644,9 @@
       <c r="AM130">
         <v>0</v>
       </c>
+      <c r="AO130">
+        <v>0.895610439712185</v>
+      </c>
       <c r="AP130">
         <v>0.03</v>
       </c>
@@ -13388,6 +13775,9 @@
       <c r="AM131">
         <v>0</v>
       </c>
+      <c r="AO131">
+        <v>0.982220964828812</v>
+      </c>
       <c r="AP131">
         <v>0.8</v>
       </c>
@@ -13477,6 +13867,9 @@
       <c r="AM132">
         <v>0</v>
       </c>
+      <c r="AO132">
+        <v>0.989874394500504</v>
+      </c>
       <c r="AP132">
         <v>2.19</v>
       </c>
@@ -13521,6 +13914,9 @@
       <c r="AM133">
         <v>0</v>
       </c>
+      <c r="AO133">
+        <v>0.976373586138954</v>
+      </c>
       <c r="AP133">
         <v>4.75</v>
       </c>
@@ -13640,6 +14036,9 @@
       <c r="AM134">
         <v>0</v>
       </c>
+      <c r="AO134">
+        <v>0.940576305644536</v>
+      </c>
       <c r="AP134">
         <v>10.75</v>
       </c>
@@ -13756,6 +14155,9 @@
       <c r="AN135">
         <v>123.74</v>
       </c>
+      <c r="AO135">
+        <v>0.970001711541853</v>
+      </c>
       <c r="AP135">
         <v>18.52</v>
       </c>
@@ -13875,6 +14277,9 @@
       <c r="AN136">
         <v>203.72</v>
       </c>
+      <c r="AO136">
+        <v>0.828628978748389</v>
+      </c>
       <c r="AP136">
         <v>21.14</v>
       </c>
@@ -13928,6 +14333,9 @@
       <c r="AN137">
         <v>429.03</v>
       </c>
+      <c r="AO137">
+        <v>0.723759141399628</v>
+      </c>
       <c r="AP137">
         <v>32.88</v>
       </c>
@@ -13981,6 +14389,9 @@
       <c r="AN138">
         <v>502.71</v>
       </c>
+      <c r="AO138">
+        <v>0.378741723048407</v>
+      </c>
       <c r="AP138">
         <v>26.64</v>
       </c>
@@ -14094,6 +14505,9 @@
       <c r="AN139">
         <v>666.98</v>
       </c>
+      <c r="AO139">
+        <v>0.154405091997514</v>
+      </c>
       <c r="AP139">
         <v>99.13</v>
       </c>
@@ -14195,6 +14609,9 @@
       <c r="AN140">
         <v>700.66</v>
       </c>
+      <c r="AO140">
+        <v>0</v>
+      </c>
       <c r="AP140">
         <v>139.34</v>
       </c>
@@ -14242,6 +14659,9 @@
       <c r="AN141">
         <v>569.49</v>
       </c>
+      <c r="AO141">
+        <v>0</v>
+      </c>
       <c r="AP141">
         <v>121.18</v>
       </c>
@@ -14286,6 +14706,9 @@
       <c r="AN142">
         <v>600.59</v>
       </c>
+      <c r="AO142">
+        <v>0</v>
+      </c>
       <c r="AQ142">
         <v>9</v>
       </c>
@@ -14369,6 +14792,9 @@
       <c r="AM143">
         <v>0</v>
       </c>
+      <c r="AO143">
+        <v>0</v>
+      </c>
       <c r="AQ143">
         <v>9</v>
       </c>
@@ -14449,6 +14875,9 @@
       <c r="AM144">
         <v>0</v>
       </c>
+      <c r="AO144">
+        <v>0</v>
+      </c>
       <c r="AQ144">
         <v>9</v>
       </c>
@@ -14529,6 +14958,9 @@
       <c r="AM145">
         <v>0</v>
       </c>
+      <c r="AO145">
+        <v>0</v>
+      </c>
       <c r="AQ145">
         <v>9</v>
       </c>
@@ -14558,6 +14990,9 @@
       <c r="AM146">
         <v>0</v>
       </c>
+      <c r="AO146">
+        <v>0.372046611873169</v>
+      </c>
       <c r="AP146">
         <v>0</v>
       </c>
@@ -14686,6 +15121,9 @@
       <c r="AM147">
         <v>0</v>
       </c>
+      <c r="AO147">
+        <v>0.739501291507127</v>
+      </c>
       <c r="AP147">
         <v>0.04</v>
       </c>
@@ -14814,6 +15252,9 @@
       <c r="AM148">
         <v>0</v>
       </c>
+      <c r="AO148">
+        <v>0.897732292941723</v>
+      </c>
       <c r="AP148">
         <v>0.32</v>
       </c>
@@ -14942,6 +15383,9 @@
       <c r="AM149">
         <v>0</v>
       </c>
+      <c r="AO149">
+        <v>0.96512023701331</v>
+      </c>
       <c r="AP149">
         <v>1.45</v>
       </c>
@@ -15031,6 +15475,9 @@
       <c r="AM150">
         <v>0</v>
       </c>
+      <c r="AO150">
+        <v>0.982179887508706</v>
+      </c>
       <c r="AP150">
         <v>1.87</v>
       </c>
@@ -15075,6 +15522,9 @@
       <c r="AM151">
         <v>0</v>
       </c>
+      <c r="AO151">
+        <v>0.9868667654959</v>
+      </c>
       <c r="AP151">
         <v>5.21</v>
       </c>
@@ -15200,6 +15650,9 @@
       <c r="AN152">
         <v>10.55</v>
       </c>
+      <c r="AO152">
+        <v>0.982437121266727</v>
+      </c>
       <c r="AP152">
         <v>8.39</v>
       </c>
@@ -15319,6 +15772,9 @@
       <c r="AN153">
         <v>109.58</v>
       </c>
+      <c r="AO153">
+        <v>0.964937051838836</v>
+      </c>
       <c r="AP153">
         <v>12.58</v>
       </c>
@@ -15441,6 +15897,9 @@
       <c r="AN154">
         <v>228.84</v>
       </c>
+      <c r="AO154">
+        <v>0.837727948395467</v>
+      </c>
       <c r="AP154">
         <v>16</v>
       </c>
@@ -15494,6 +15953,9 @@
       <c r="AN155">
         <v>412.95</v>
       </c>
+      <c r="AO155">
+        <v>0.841817206549362</v>
+      </c>
       <c r="AP155">
         <v>26.69</v>
       </c>
@@ -15547,6 +16009,9 @@
       <c r="AN156">
         <v>573.96</v>
       </c>
+      <c r="AO156">
+        <v>0.707074678856153</v>
+      </c>
       <c r="AP156">
         <v>32.18</v>
       </c>
@@ -15657,6 +16122,9 @@
       <c r="AN157">
         <v>719.32</v>
       </c>
+      <c r="AO157">
+        <v>0.35951634622328</v>
+      </c>
       <c r="AP157">
         <v>46.17</v>
       </c>
@@ -15761,6 +16229,9 @@
       <c r="AN158">
         <v>728.93</v>
       </c>
+      <c r="AO158">
+        <v>0</v>
+      </c>
       <c r="AP158">
         <v>145.13</v>
       </c>
@@ -15808,6 +16279,9 @@
       <c r="AN159">
         <v>643.37</v>
       </c>
+      <c r="AO159">
+        <v>0</v>
+      </c>
       <c r="AP159">
         <v>151.62</v>
       </c>
@@ -15852,6 +16326,9 @@
       <c r="AN160">
         <v>570.39</v>
       </c>
+      <c r="AO160">
+        <v>0</v>
+      </c>
       <c r="AQ160">
         <v>9</v>
       </c>
@@ -15935,6 +16412,9 @@
       <c r="AM161">
         <v>0</v>
       </c>
+      <c r="AO161">
+        <v>0</v>
+      </c>
       <c r="AQ161">
         <v>9</v>
       </c>
@@ -16015,6 +16495,9 @@
       <c r="AM162">
         <v>0</v>
       </c>
+      <c r="AO162">
+        <v>0</v>
+      </c>
       <c r="AQ162">
         <v>9</v>
       </c>
@@ -16095,6 +16578,9 @@
       <c r="AM163">
         <v>0</v>
       </c>
+      <c r="AO163">
+        <v>0</v>
+      </c>
       <c r="AQ163">
         <v>9</v>
       </c>
@@ -16124,6 +16610,9 @@
       <c r="AM164">
         <v>0</v>
       </c>
+      <c r="AO164">
+        <v>0.343303131582766</v>
+      </c>
       <c r="AP164">
         <v>0</v>
       </c>
@@ -16171,6 +16660,9 @@
       <c r="AM165">
         <v>0</v>
       </c>
+      <c r="AO165">
+        <v>0.750836717174127</v>
+      </c>
       <c r="AP165">
         <v>0.03</v>
       </c>
@@ -16218,6 +16710,9 @@
       <c r="AM166">
         <v>0</v>
       </c>
+      <c r="AO166">
+        <v>0.817234967991759</v>
+      </c>
       <c r="AP166">
         <v>0.28</v>
       </c>
@@ -16265,6 +16760,9 @@
       <c r="AM167">
         <v>0</v>
       </c>
+      <c r="AO167">
+        <v>0.900968510674936</v>
+      </c>
       <c r="AP167">
         <v>0.76</v>
       </c>
@@ -16354,6 +16852,9 @@
       <c r="AM168">
         <v>0</v>
       </c>
+      <c r="AO168">
+        <v>0.91360921404333</v>
+      </c>
       <c r="AP168">
         <v>0.72</v>
       </c>
@@ -16395,6 +16896,9 @@
       <c r="AM169">
         <v>0</v>
       </c>
+      <c r="AO169">
+        <v>0.924014273349758</v>
+      </c>
       <c r="AP169">
         <v>3.59</v>
       </c>
@@ -16448,6 +16952,9 @@
       <c r="AN170">
         <v>127.72</v>
       </c>
+      <c r="AO170">
+        <v>0.866060792411396</v>
+      </c>
       <c r="AP170">
         <v>5.79</v>
       </c>
@@ -16501,6 +17008,9 @@
       <c r="AN171">
         <v>177.69</v>
       </c>
+      <c r="AO171">
+        <v>0.75850471362725</v>
+      </c>
       <c r="AP171">
         <v>6.88</v>
       </c>
@@ -16554,6 +17064,9 @@
       <c r="AN172">
         <v>282.76</v>
       </c>
+      <c r="AO172">
+        <v>0.726879058452995</v>
+      </c>
       <c r="AP172">
         <v>8.29</v>
       </c>
@@ -16601,6 +17114,9 @@
       <c r="AN173">
         <v>525.61</v>
       </c>
+      <c r="AO173">
+        <v>0.543701270805572</v>
+      </c>
       <c r="AP173">
         <v>20.26</v>
       </c>
@@ -16654,6 +17170,9 @@
       <c r="AN174">
         <v>331.32</v>
       </c>
+      <c r="AO174">
+        <v>0.0979938778034154</v>
+      </c>
       <c r="AP174">
         <v>40.85</v>
       </c>
@@ -16704,6 +17223,9 @@
       <c r="AN175">
         <v>532.17</v>
       </c>
+      <c r="AO175">
+        <v>0</v>
+      </c>
       <c r="AP175">
         <v>85.26</v>
       </c>
@@ -16751,6 +17273,9 @@
       <c r="AN176">
         <v>612.64</v>
       </c>
+      <c r="AO176">
+        <v>0</v>
+      </c>
       <c r="AP176">
         <v>83.29</v>
       </c>
@@ -16798,6 +17323,9 @@
       <c r="AN177">
         <v>508.18</v>
       </c>
+      <c r="AO177">
+        <v>0</v>
+      </c>
       <c r="AP177">
         <v>73.67</v>
       </c>
@@ -16842,6 +17370,9 @@
       <c r="AN178">
         <v>446.26</v>
       </c>
+      <c r="AO178">
+        <v>0</v>
+      </c>
       <c r="AQ178">
         <v>9</v>
       </c>
@@ -16871,6 +17402,9 @@
       <c r="AM179">
         <v>0</v>
       </c>
+      <c r="AO179">
+        <v>0</v>
+      </c>
       <c r="AQ179">
         <v>9</v>
       </c>
@@ -16897,6 +17431,9 @@
       <c r="AM180">
         <v>0</v>
       </c>
+      <c r="AO180">
+        <v>0</v>
+      </c>
       <c r="AQ180">
         <v>9</v>
       </c>
@@ -16921,6 +17458,9 @@
         <v>36222</v>
       </c>
       <c r="AM181">
+        <v>0</v>
+      </c>
+      <c r="AO181">
         <v>0</v>
       </c>
       <c r="AQ181">

</xml_diff>

<commit_message>
Progress with fitting Oat model
</commit_message>
<xml_diff>
--- a/Prototypes/Oats/Observed.xlsx
+++ b/Prototypes/Oats/Observed.xlsx
@@ -17558,7 +17558,7 @@
         <v>0</v>
       </c>
       <c r="AH186">
-        <v>18.7568970210553</v>
+        <v>1.87568970210553</v>
       </c>
       <c r="AI186">
         <v>53.3512025587154</v>
@@ -17601,7 +17601,7 @@
         <v>0</v>
       </c>
       <c r="AH188">
-        <v>34.4338625</v>
+        <v>3.44338625</v>
       </c>
       <c r="AI188">
         <v>197.625</v>
@@ -17664,7 +17664,7 @@
         <v>0</v>
       </c>
       <c r="AH191">
-        <v>60.6146841736801</v>
+        <v>6.06146841736801</v>
       </c>
       <c r="AI191">
         <v>498.949219844169</v>
@@ -17707,7 +17707,7 @@
         <v>0</v>
       </c>
       <c r="AH193">
-        <v>76.1638350160525</v>
+        <v>7.61638350160525</v>
       </c>
       <c r="AI193">
         <v>665.067103645806</v>
@@ -17801,7 +17801,7 @@
         <v>400</v>
       </c>
       <c r="AH198">
-        <v>17.9867970348076</v>
+        <v>1.79867970348076</v>
       </c>
       <c r="AI198">
         <v>46.6335848773505</v>
@@ -17844,7 +17844,7 @@
         <v>400</v>
       </c>
       <c r="AH200">
-        <v>91.7196875</v>
+        <v>9.17196875</v>
       </c>
       <c r="AI200">
         <v>306.75</v>
@@ -17907,7 +17907,7 @@
         <v>400</v>
       </c>
       <c r="AH203">
-        <v>199.704282398221</v>
+        <v>19.9704282398221</v>
       </c>
       <c r="AI203">
         <v>895.812286745283</v>
@@ -17950,7 +17950,7 @@
         <v>400</v>
       </c>
       <c r="AH205">
-        <v>228.536831355868</v>
+        <v>22.8536831355868</v>
       </c>
       <c r="AI205">
         <v>1083.93398948241</v>
@@ -18044,7 +18044,7 @@
         <v>0</v>
       </c>
       <c r="AH210">
-        <v>26.784627615825</v>
+        <v>2.6784627615825</v>
       </c>
       <c r="AI210">
         <v>103.165708792433</v>
@@ -18087,7 +18087,7 @@
         <v>0</v>
       </c>
       <c r="AH212">
-        <v>47.7519875</v>
+        <v>4.77519875</v>
       </c>
       <c r="AI212">
         <v>379.875</v>
@@ -18150,7 +18150,7 @@
         <v>0</v>
       </c>
       <c r="AH215">
-        <v>55.4133727708923</v>
+        <v>5.54133727708923</v>
       </c>
       <c r="AI215">
         <v>609.822410350116</v>
@@ -18284,7 +18284,7 @@
         <v>400</v>
       </c>
       <c r="AH222">
-        <v>39.6189411704857</v>
+        <v>3.96189411704857</v>
       </c>
       <c r="AI222">
         <v>98.9996733880507</v>
@@ -18327,7 +18327,7 @@
         <v>400</v>
       </c>
       <c r="AH224">
-        <v>144.4308125</v>
+        <v>14.44308125</v>
       </c>
       <c r="AI224">
         <v>538.375</v>
@@ -18390,7 +18390,7 @@
         <v>400</v>
       </c>
       <c r="AH227">
-        <v>242.831886393812</v>
+        <v>24.2831886393812</v>
       </c>
       <c r="AI227">
         <v>1177.6120684649</v>
@@ -18557,6 +18557,9 @@
       <c r="E236">
         <v>400</v>
       </c>
+      <c r="AH236">
+        <v>3.27126</v>
+      </c>
       <c r="AI236">
         <v>50.3</v>
       </c>
@@ -18611,6 +18614,9 @@
       <c r="E239">
         <v>400</v>
       </c>
+      <c r="AH239">
+        <v>12.7629350296989</v>
+      </c>
       <c r="AI239">
         <v>326.709856011823</v>
       </c>
@@ -18648,6 +18654,9 @@
       <c r="E241">
         <v>400</v>
       </c>
+      <c r="AH241">
+        <v>16.4410330801934</v>
+      </c>
       <c r="AI241">
         <v>493.399307720302</v>
       </c>
@@ -18753,6 +18762,9 @@
       <c r="E247">
         <v>400</v>
       </c>
+      <c r="AH247">
+        <v>20.1199599446612</v>
+      </c>
       <c r="AI247">
         <v>1194.30360373165</v>
       </c>
@@ -18926,6 +18938,9 @@
       <c r="E257">
         <v>400</v>
       </c>
+      <c r="AH257">
+        <v>6.319725</v>
+      </c>
       <c r="AI257">
         <v>103.95</v>
       </c>
@@ -18980,6 +18995,9 @@
       <c r="E260">
         <v>400</v>
       </c>
+      <c r="AH260">
+        <v>13.3791837436829</v>
+      </c>
       <c r="AI260">
         <v>443.641802204155</v>
       </c>
@@ -19017,6 +19035,9 @@
       <c r="E262">
         <v>400</v>
       </c>
+      <c r="AH262">
+        <v>16.850662867467</v>
+      </c>
       <c r="AI262">
         <v>697.328104091977</v>
       </c>
@@ -19084,6 +19105,9 @@
       </c>
       <c r="E266">
         <v>400</v>
+      </c>
+      <c r="AH266">
+        <v>17.7518187225726</v>
       </c>
       <c r="AI266">
         <v>1276.7247244337</v>

</xml_diff>

<commit_message>
Removed some zeros and changed harvesting rule for rainout shelter 9899
</commit_message>
<xml_diff>
--- a/Prototypes/Oats/Observed.xlsx
+++ b/Prototypes/Oats/Observed.xlsx
@@ -998,10 +998,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CA904"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="BD1" sqref="BD1"/>
-      <selection pane="bottomLeft" activeCell="BI304" sqref="BI304"/>
+      <selection pane="bottomLeft" activeCell="AO1" sqref="AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11246,9 +11246,6 @@
       <c r="AN102">
         <v>476.6</v>
       </c>
-      <c r="AO102">
-        <v>0</v>
-      </c>
       <c r="AP102">
         <v>31.32</v>
       </c>
@@ -11353,9 +11350,6 @@
       <c r="AN103">
         <v>634.51</v>
       </c>
-      <c r="AO103">
-        <v>0</v>
-      </c>
       <c r="AP103">
         <v>117.62</v>
       </c>
@@ -11376,9 +11370,6 @@
       </c>
       <c r="AZ103">
         <v>85.51</v>
-      </c>
-      <c r="BL103">
-        <v>0</v>
       </c>
       <c r="CA103" t="s">
         <v>182</v>
@@ -11454,9 +11445,6 @@
       <c r="AN104">
         <v>577.24</v>
       </c>
-      <c r="AO104">
-        <v>0</v>
-      </c>
       <c r="AP104">
         <v>94.95</v>
       </c>
@@ -11477,9 +11465,6 @@
       </c>
       <c r="AZ104">
         <v>83.69</v>
-      </c>
-      <c r="BL104">
-        <v>0</v>
       </c>
       <c r="CA104" t="s">
         <v>182</v>
@@ -11501,9 +11486,6 @@
       <c r="AN105">
         <v>574.52</v>
       </c>
-      <c r="AO105">
-        <v>0</v>
-      </c>
       <c r="AP105">
         <v>92.45</v>
       </c>
@@ -11524,9 +11506,6 @@
       </c>
       <c r="AZ105">
         <v>71.760000000000005</v>
-      </c>
-      <c r="BL105">
-        <v>0</v>
       </c>
       <c r="CA105" t="s">
         <v>182</v>
@@ -11545,9 +11524,6 @@
       <c r="AN106">
         <v>507.33</v>
       </c>
-      <c r="AO106">
-        <v>0</v>
-      </c>
       <c r="AQ106">
         <v>9</v>
       </c>
@@ -11559,9 +11535,6 @@
       </c>
       <c r="BA106" t="s">
         <v>165</v>
-      </c>
-      <c r="BL106">
-        <v>0</v>
       </c>
       <c r="CA106" t="s">
         <v>182</v>
@@ -11631,9 +11604,6 @@
       <c r="AM107">
         <v>0</v>
       </c>
-      <c r="AO107">
-        <v>0</v>
-      </c>
       <c r="AQ107">
         <v>9</v>
       </c>
@@ -11641,9 +11611,6 @@
         <v>0</v>
       </c>
       <c r="AY107">
-        <v>0</v>
-      </c>
-      <c r="BL107">
         <v>0</v>
       </c>
       <c r="CA107" t="s">
@@ -11714,9 +11681,6 @@
       <c r="AM108">
         <v>0</v>
       </c>
-      <c r="AO108">
-        <v>0</v>
-      </c>
       <c r="AQ108">
         <v>9</v>
       </c>
@@ -11724,9 +11688,6 @@
         <v>0</v>
       </c>
       <c r="AY108">
-        <v>0</v>
-      </c>
-      <c r="BL108">
         <v>0</v>
       </c>
       <c r="CA108" t="s">
@@ -11797,9 +11758,6 @@
       <c r="AM109">
         <v>0</v>
       </c>
-      <c r="AO109">
-        <v>0</v>
-      </c>
       <c r="AQ109">
         <v>9</v>
       </c>
@@ -11807,9 +11765,6 @@
         <v>0</v>
       </c>
       <c r="AY109">
-        <v>0</v>
-      </c>
-      <c r="BL109">
         <v>0</v>
       </c>
       <c r="CA109" t="s">
@@ -12955,9 +12910,6 @@
       <c r="AN121">
         <v>686.02</v>
       </c>
-      <c r="AO121">
-        <v>0</v>
-      </c>
       <c r="AP121">
         <v>125.63</v>
       </c>
@@ -12978,9 +12930,6 @@
       </c>
       <c r="AZ121">
         <v>86.62</v>
-      </c>
-      <c r="BL121">
-        <v>0</v>
       </c>
       <c r="CA121" t="s">
         <v>183</v>
@@ -13056,9 +13005,6 @@
       <c r="AN122">
         <v>661.07</v>
       </c>
-      <c r="AO122">
-        <v>0</v>
-      </c>
       <c r="AP122">
         <v>123.88</v>
       </c>
@@ -13079,9 +13025,6 @@
       </c>
       <c r="AZ122">
         <v>101.93</v>
-      </c>
-      <c r="BL122">
-        <v>0</v>
       </c>
       <c r="CA122" t="s">
         <v>183</v>
@@ -13103,9 +13046,6 @@
       <c r="AN123">
         <v>654.45000000000005</v>
       </c>
-      <c r="AO123">
-        <v>0</v>
-      </c>
       <c r="AP123">
         <v>115.2</v>
       </c>
@@ -13126,9 +13066,6 @@
       </c>
       <c r="AZ123">
         <v>73.13</v>
-      </c>
-      <c r="BL123">
-        <v>0</v>
       </c>
       <c r="CA123" t="s">
         <v>183</v>
@@ -13147,9 +13084,6 @@
       <c r="AN124">
         <v>543.05999999999995</v>
       </c>
-      <c r="AO124">
-        <v>0</v>
-      </c>
       <c r="AQ124">
         <v>9</v>
       </c>
@@ -13161,9 +13095,6 @@
       </c>
       <c r="BA124" t="s">
         <v>165</v>
-      </c>
-      <c r="BL124">
-        <v>0</v>
       </c>
       <c r="CA124" t="s">
         <v>183</v>
@@ -13233,9 +13164,6 @@
       <c r="AM125">
         <v>0</v>
       </c>
-      <c r="AO125">
-        <v>0</v>
-      </c>
       <c r="AQ125">
         <v>9</v>
       </c>
@@ -13243,9 +13171,6 @@
         <v>0</v>
       </c>
       <c r="AY125">
-        <v>0</v>
-      </c>
-      <c r="BL125">
         <v>0</v>
       </c>
       <c r="CA125" t="s">
@@ -13316,9 +13241,6 @@
       <c r="AM126">
         <v>0</v>
       </c>
-      <c r="AO126">
-        <v>0</v>
-      </c>
       <c r="AQ126">
         <v>9</v>
       </c>
@@ -13326,9 +13248,6 @@
         <v>0</v>
       </c>
       <c r="AY126">
-        <v>0</v>
-      </c>
-      <c r="BL126">
         <v>0</v>
       </c>
       <c r="CA126" t="s">
@@ -13399,9 +13318,6 @@
       <c r="AM127">
         <v>0</v>
       </c>
-      <c r="AO127">
-        <v>0</v>
-      </c>
       <c r="AQ127">
         <v>9</v>
       </c>
@@ -13409,9 +13325,6 @@
         <v>0</v>
       </c>
       <c r="AY127">
-        <v>0</v>
-      </c>
-      <c r="BL127">
         <v>0</v>
       </c>
       <c r="CA127" t="s">
@@ -14658,9 +14571,6 @@
       <c r="AN140">
         <v>700.66</v>
       </c>
-      <c r="AO140">
-        <v>0</v>
-      </c>
       <c r="AP140">
         <v>139.34</v>
       </c>
@@ -14681,9 +14591,6 @@
       </c>
       <c r="AZ140">
         <v>102.15</v>
-      </c>
-      <c r="BL140">
-        <v>0</v>
       </c>
       <c r="CA140" t="s">
         <v>184</v>
@@ -14705,9 +14612,6 @@
       <c r="AN141">
         <v>569.49</v>
       </c>
-      <c r="AO141">
-        <v>0</v>
-      </c>
       <c r="AP141">
         <v>121.18</v>
       </c>
@@ -14728,9 +14632,6 @@
       </c>
       <c r="AZ141">
         <v>93.38</v>
-      </c>
-      <c r="BL141">
-        <v>0</v>
       </c>
       <c r="CA141" t="s">
         <v>184</v>
@@ -14749,9 +14650,6 @@
       <c r="AN142">
         <v>600.59</v>
       </c>
-      <c r="AO142">
-        <v>0</v>
-      </c>
       <c r="AQ142">
         <v>9</v>
       </c>
@@ -14763,9 +14661,6 @@
       </c>
       <c r="BA142" t="s">
         <v>165</v>
-      </c>
-      <c r="BL142">
-        <v>0</v>
       </c>
       <c r="CA142" t="s">
         <v>184</v>
@@ -14835,9 +14730,6 @@
       <c r="AM143">
         <v>0</v>
       </c>
-      <c r="AO143">
-        <v>0</v>
-      </c>
       <c r="AQ143">
         <v>9</v>
       </c>
@@ -14845,9 +14737,6 @@
         <v>0</v>
       </c>
       <c r="AY143">
-        <v>0</v>
-      </c>
-      <c r="BL143">
         <v>0</v>
       </c>
       <c r="CA143" t="s">
@@ -14918,9 +14807,6 @@
       <c r="AM144">
         <v>0</v>
       </c>
-      <c r="AO144">
-        <v>0</v>
-      </c>
       <c r="AQ144">
         <v>9</v>
       </c>
@@ -14928,9 +14814,6 @@
         <v>0</v>
       </c>
       <c r="AY144">
-        <v>0</v>
-      </c>
-      <c r="BL144">
         <v>0</v>
       </c>
       <c r="CA144" t="s">
@@ -15001,9 +14884,6 @@
       <c r="AM145">
         <v>0</v>
       </c>
-      <c r="AO145">
-        <v>0</v>
-      </c>
       <c r="AQ145">
         <v>9</v>
       </c>
@@ -15011,9 +14891,6 @@
         <v>0</v>
       </c>
       <c r="AY145">
-        <v>0</v>
-      </c>
-      <c r="BL145">
         <v>0</v>
       </c>
       <c r="CA145" t="s">
@@ -16272,9 +16149,6 @@
       <c r="AN158">
         <v>728.93</v>
       </c>
-      <c r="AO158">
-        <v>0</v>
-      </c>
       <c r="AP158">
         <v>145.13</v>
       </c>
@@ -16295,9 +16169,6 @@
       </c>
       <c r="AZ158">
         <v>107.86</v>
-      </c>
-      <c r="BL158">
-        <v>0</v>
       </c>
       <c r="CA158" t="s">
         <v>185</v>
@@ -16319,9 +16190,6 @@
       <c r="AN159">
         <v>643.37</v>
       </c>
-      <c r="AO159">
-        <v>0</v>
-      </c>
       <c r="AP159">
         <v>151.62</v>
       </c>
@@ -16342,9 +16210,6 @@
       </c>
       <c r="AZ159">
         <v>98.39</v>
-      </c>
-      <c r="BL159">
-        <v>0</v>
       </c>
       <c r="CA159" t="s">
         <v>185</v>
@@ -16363,9 +16228,6 @@
       <c r="AN160">
         <v>570.39</v>
       </c>
-      <c r="AO160">
-        <v>0</v>
-      </c>
       <c r="AQ160">
         <v>9</v>
       </c>
@@ -16377,9 +16239,6 @@
       </c>
       <c r="BA160" t="s">
         <v>165</v>
-      </c>
-      <c r="BL160">
-        <v>0</v>
       </c>
       <c r="CA160" t="s">
         <v>185</v>
@@ -16449,9 +16308,6 @@
       <c r="AM161">
         <v>0</v>
       </c>
-      <c r="AO161">
-        <v>0</v>
-      </c>
       <c r="AQ161">
         <v>9</v>
       </c>
@@ -16459,9 +16315,6 @@
         <v>0</v>
       </c>
       <c r="AY161">
-        <v>0</v>
-      </c>
-      <c r="BL161">
         <v>0</v>
       </c>
       <c r="CA161" t="s">
@@ -16532,9 +16385,6 @@
       <c r="AM162">
         <v>0</v>
       </c>
-      <c r="AO162">
-        <v>0</v>
-      </c>
       <c r="AQ162">
         <v>9</v>
       </c>
@@ -16542,9 +16392,6 @@
         <v>0</v>
       </c>
       <c r="AY162">
-        <v>0</v>
-      </c>
-      <c r="BL162">
         <v>0</v>
       </c>
       <c r="CA162" t="s">
@@ -16615,9 +16462,6 @@
       <c r="AM163">
         <v>0</v>
       </c>
-      <c r="AO163">
-        <v>0</v>
-      </c>
       <c r="AQ163">
         <v>9</v>
       </c>
@@ -16625,9 +16469,6 @@
         <v>0</v>
       </c>
       <c r="AY163">
-        <v>0</v>
-      </c>
-      <c r="BL163">
         <v>0</v>
       </c>
       <c r="CA163" t="s">
@@ -17260,9 +17101,6 @@
       <c r="AN175">
         <v>532.16999999999996</v>
       </c>
-      <c r="AO175">
-        <v>0</v>
-      </c>
       <c r="AP175">
         <v>85.26</v>
       </c>
@@ -17283,9 +17121,6 @@
       </c>
       <c r="AZ175">
         <v>81.040000000000006</v>
-      </c>
-      <c r="BL175">
-        <v>0</v>
       </c>
       <c r="CA175" t="s">
         <v>188</v>
@@ -17307,9 +17142,6 @@
       <c r="AN176">
         <v>612.64</v>
       </c>
-      <c r="AO176">
-        <v>0</v>
-      </c>
       <c r="AP176">
         <v>83.29</v>
       </c>
@@ -17330,9 +17162,6 @@
       </c>
       <c r="AZ176">
         <v>74.819999999999993</v>
-      </c>
-      <c r="BL176">
-        <v>0</v>
       </c>
       <c r="CA176" t="s">
         <v>188</v>
@@ -17354,9 +17183,6 @@
       <c r="AN177">
         <v>508.18</v>
       </c>
-      <c r="AO177">
-        <v>0</v>
-      </c>
       <c r="AP177">
         <v>73.67</v>
       </c>
@@ -17377,9 +17203,6 @@
       </c>
       <c r="AZ177">
         <v>56.26</v>
-      </c>
-      <c r="BL177">
-        <v>0</v>
       </c>
       <c r="CA177" t="s">
         <v>188</v>
@@ -17398,9 +17221,6 @@
       <c r="AN178">
         <v>446.26</v>
       </c>
-      <c r="AO178">
-        <v>0</v>
-      </c>
       <c r="AQ178">
         <v>9</v>
       </c>
@@ -17412,9 +17232,6 @@
       </c>
       <c r="BA178" t="s">
         <v>165</v>
-      </c>
-      <c r="BL178">
-        <v>0</v>
       </c>
       <c r="CA178" t="s">
         <v>188</v>
@@ -17430,9 +17247,6 @@
       <c r="AM179">
         <v>0</v>
       </c>
-      <c r="AO179">
-        <v>0</v>
-      </c>
       <c r="AQ179">
         <v>9</v>
       </c>
@@ -17440,9 +17254,6 @@
         <v>0</v>
       </c>
       <c r="AY179">
-        <v>0</v>
-      </c>
-      <c r="BL179">
         <v>0</v>
       </c>
       <c r="CA179" t="s">
@@ -17459,9 +17270,6 @@
       <c r="AM180">
         <v>0</v>
       </c>
-      <c r="AO180">
-        <v>0</v>
-      </c>
       <c r="AQ180">
         <v>9</v>
       </c>
@@ -17469,9 +17277,6 @@
         <v>0</v>
       </c>
       <c r="AY180">
-        <v>0</v>
-      </c>
-      <c r="BL180">
         <v>0</v>
       </c>
       <c r="CA180" t="s">
@@ -17488,9 +17293,6 @@
       <c r="AM181">
         <v>0</v>
       </c>
-      <c r="AO181">
-        <v>0</v>
-      </c>
       <c r="AQ181">
         <v>9</v>
       </c>
@@ -17498,9 +17300,6 @@
         <v>0</v>
       </c>
       <c r="AY181">
-        <v>0</v>
-      </c>
-      <c r="BL181">
         <v>0</v>
       </c>
       <c r="CA181" t="s">
@@ -20603,9 +20402,6 @@
       <c r="BI309">
         <v>21.5713268826734</v>
       </c>
-      <c r="BL309">
-        <v>0</v>
-      </c>
       <c r="BM309">
         <v>393.62206320673602</v>
       </c>
@@ -20908,9 +20704,6 @@
       <c r="BI316">
         <v>21.5713268826734</v>
       </c>
-      <c r="BL316">
-        <v>0</v>
-      </c>
       <c r="BM316">
         <v>393.62206320673602</v>
       </c>
@@ -21140,9 +20933,6 @@
       <c r="BI321">
         <v>21.5713268826734</v>
       </c>
-      <c r="BL321">
-        <v>0</v>
-      </c>
       <c r="BM321">
         <v>393.62206320673602</v>
       </c>
@@ -21328,9 +21118,6 @@
       <c r="BI325">
         <v>15.803954928042501</v>
       </c>
-      <c r="BL325">
-        <v>0</v>
-      </c>
       <c r="BM325">
         <v>400.10814606996797</v>
       </c>
@@ -21633,9 +21420,6 @@
       <c r="BI332">
         <v>15.803954928042501</v>
       </c>
-      <c r="BL332">
-        <v>0</v>
-      </c>
       <c r="BM332">
         <v>400.10814606996797</v>
       </c>
@@ -21865,9 +21649,6 @@
       <c r="BI337">
         <v>15.803954928042501</v>
       </c>
-      <c r="BL337">
-        <v>0</v>
-      </c>
       <c r="BM337">
         <v>400.10814606996797</v>
       </c>
@@ -22053,9 +21834,6 @@
       <c r="BI341">
         <v>23.6223812705908</v>
       </c>
-      <c r="BL341">
-        <v>0</v>
-      </c>
       <c r="BM341">
         <v>405.42779726674098</v>
       </c>
@@ -22358,9 +22136,6 @@
       <c r="BI348">
         <v>23.6223812705908</v>
       </c>
-      <c r="BL348">
-        <v>0</v>
-      </c>
       <c r="BM348">
         <v>405.42779726674098</v>
       </c>
@@ -22589,9 +22364,6 @@
       </c>
       <c r="BI353">
         <v>23.6223812705908</v>
-      </c>
-      <c r="BL353">
-        <v>0</v>
       </c>
       <c r="BM353">
         <v>405.42779726674098</v>

</xml_diff>